<commit_message>
edits to ensure all tests in pytest run prior to PR, pregnancy supervisor and labour registered in symptom manager test file
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_AntenatalCare.xlsx
+++ b/resources/ResourceFile_AntenatalCare.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>parameter_name</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t>DHS 2015- seeks ANC at least once</t>
+  </si>
+  <si>
+    <t>odds_first_anc</t>
+  </si>
+  <si>
+    <t>or_anc_unmarried</t>
+  </si>
+  <si>
+    <t>or_anc_wealth_4</t>
+  </si>
+  <si>
+    <t>or_anc_wealth_5</t>
+  </si>
+  <si>
+    <t>or_anc_urban</t>
   </si>
 </sst>
 </file>
@@ -369,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,6 +417,46 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>